<commit_message>
feat: update lab report
</commit_message>
<xml_diff>
--- a/report/EE4204_SocketProgramming_NGTZEKEAN.xlsx
+++ b/report/EE4204_SocketProgramming_NGTZEKEAN.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ngtze\Github\EE4204-Computer-Network-Lab\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ngtze\Github\EE4204-Computer-Network-Lab\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{20E56716-37F9-41C1-8A3A-3E8A84C3A3B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1EB894C-A938-40C0-86A1-8D2C91C3ED74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10718" yWindow="0" windowWidth="10965" windowHeight="13583" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="210" yWindow="330" windowWidth="20445" windowHeight="12870" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,8 @@
     <t>Data rate (kbytes/s) Fixed</t>
   </si>
   <si>
-    <t>As the data unit size increassed, so did the data rate of the transmission. This is because the more data would be transmitted in with less time spent on defragmentation at the end point. This speeds up the process of the overall transmission.
+    <t>Report:
+As the data unit size increassed, so did the data rate of the transmission. This is because the more data would be transmitted in with less time spent on defragmentation at the end point. This speeds up the process of the overall transmission.
 What was interesting is that as the DU increased, the growth in data rate and the decrease in time was not linear but exponential for both protocol. This indicated that the performance improvement for both is favourable for increased DU. Another observation was that the difference in the performance between the 2 protocol was not substantial. While the protocol that used the varying ACK has slightly poorer data rate, the difference is minor. This could be due to the small RTT as there is minimal hops for the transmission of the message of the client to the server and hence the delay of the ACK did not substantially affect the tranmission. It is also important to note that for every 6 packets, there will be 3 ACK for both protocol, what differs the the size of the window that is allocated for the tranmission, where the fixed-batch always has 2, while the vary-batch will change between [1,2,3].
 The assumptions made are
 1. The hops taken by the packet is the same for a fair comparison of different DUs
@@ -59,7 +60,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -546,10 +547,10 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3385,7 +3386,7 @@
   <dimension ref="A1:W36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="64" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="Y14" sqref="Y14"/>
+      <selection activeCell="O1" sqref="O1:W24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3397,12 +3398,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
       <c r="O1" s="3" t="s">
         <v>8</v>
       </c>
@@ -3445,7 +3446,7 @@
       <c r="B3">
         <v>59793</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="1">
         <v>1216.7144780000001</v>
       </c>
       <c r="D3">
@@ -3468,7 +3469,7 @@
       <c r="B4">
         <v>59793</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <v>2115.8923340000001</v>
       </c>
       <c r="D4">
@@ -3491,7 +3492,7 @@
       <c r="B5">
         <v>59793</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
         <v>3210.7072750000002</v>
       </c>
       <c r="D5">
@@ -3514,7 +3515,7 @@
       <c r="B6">
         <v>59793</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="1">
         <v>4828.2460940000001</v>
       </c>
       <c r="D6">
@@ -3537,7 +3538,7 @@
       <c r="B7">
         <v>59793</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="1">
         <v>6590.939453</v>
       </c>
       <c r="D7">
@@ -3560,7 +3561,7 @@
       <c r="B8">
         <v>59793</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="1">
         <v>6511.9799800000001</v>
       </c>
       <c r="D8">
@@ -3583,7 +3584,7 @@
       <c r="B9">
         <v>59793</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="1">
         <v>8399.0732420000004</v>
       </c>
       <c r="D9">
@@ -3606,7 +3607,7 @@
       <c r="B10">
         <v>59793</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="1">
         <v>11155.410156</v>
       </c>
       <c r="D10">
@@ -3629,7 +3630,7 @@
       <c r="B11">
         <v>59793</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="1">
         <v>15008.283203000001</v>
       </c>
       <c r="D11">
@@ -3652,7 +3653,7 @@
       <c r="B12">
         <v>59793</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="1">
         <v>21601.517577999999</v>
       </c>
       <c r="D12">
@@ -3675,7 +3676,7 @@
       <c r="B13">
         <v>59793</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="1">
         <v>40926.078125</v>
       </c>
       <c r="D13">
@@ -3698,7 +3699,7 @@
       <c r="B14">
         <v>59793</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="1">
         <v>64224.488280999998</v>
       </c>
       <c r="D14">
@@ -3721,7 +3722,7 @@
       <c r="B15">
         <v>59793</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="1">
         <v>101344.070312</v>
       </c>
       <c r="D15">
@@ -3744,7 +3745,7 @@
       <c r="B16">
         <v>59793</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="1">
         <v>147273.40625</v>
       </c>
       <c r="D16">
@@ -3767,7 +3768,7 @@
       <c r="B17">
         <v>59793</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="1">
         <v>193504.859375</v>
       </c>
       <c r="D17">
@@ -3790,7 +3791,7 @@
       <c r="B18">
         <v>59793</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="1">
         <v>854185.6875</v>
       </c>
       <c r="D18">
@@ -3813,7 +3814,7 @@
       <c r="B19">
         <v>59793</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="1">
         <v>747412.5</v>
       </c>
       <c r="D19">
@@ -3841,12 +3842,12 @@
       <c r="W20" s="3"/>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
       <c r="O21" s="3"/>
       <c r="P21" s="3"/>
       <c r="Q21" s="3"/>
@@ -3887,7 +3888,7 @@
       <c r="B23">
         <v>59793</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="1">
         <v>1130.6016850000001</v>
       </c>
       <c r="D23">
@@ -3910,7 +3911,7 @@
       <c r="B24">
         <v>59793</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24" s="1">
         <v>2262.4011230000001</v>
       </c>
       <c r="D24">
@@ -3933,7 +3934,7 @@
       <c r="B25">
         <v>59793</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25" s="1">
         <v>3495.6445309999999</v>
       </c>
       <c r="D25">
@@ -3947,7 +3948,7 @@
       <c r="B26">
         <v>59793</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C26" s="1">
         <v>4491.9990230000003</v>
       </c>
       <c r="D26">
@@ -3961,7 +3962,7 @@
       <c r="B27">
         <v>59793</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C27" s="1">
         <v>5763.1806640000004</v>
       </c>
       <c r="D27">
@@ -3975,7 +3976,7 @@
       <c r="B28">
         <v>59793</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C28" s="1">
         <v>6825.6845700000003</v>
       </c>
       <c r="D28">
@@ -3989,7 +3990,7 @@
       <c r="B29">
         <v>59793</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C29" s="1">
         <v>7963.9052730000003</v>
       </c>
       <c r="D29">
@@ -4003,7 +4004,7 @@
       <c r="B30">
         <v>59793</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C30" s="1">
         <v>12315.756836</v>
       </c>
       <c r="D30">
@@ -4017,7 +4018,7 @@
       <c r="B31">
         <v>59793</v>
       </c>
-      <c r="C31" s="2">
+      <c r="C31" s="1">
         <v>13889.199219</v>
       </c>
       <c r="D31">
@@ -4031,7 +4032,7 @@
       <c r="B32">
         <v>59793</v>
       </c>
-      <c r="C32" s="2">
+      <c r="C32" s="1">
         <v>19668.75</v>
       </c>
       <c r="D32">
@@ -4045,7 +4046,7 @@
       <c r="B33">
         <v>59793</v>
       </c>
-      <c r="C33" s="2">
+      <c r="C33" s="1">
         <v>43485.816405999998</v>
       </c>
       <c r="D33">
@@ -4059,7 +4060,7 @@
       <c r="B34">
         <v>59793</v>
       </c>
-      <c r="C34" s="2">
+      <c r="C34" s="1">
         <v>55210.527344000002</v>
       </c>
       <c r="D34">
@@ -4073,7 +4074,7 @@
       <c r="B35">
         <v>59793</v>
       </c>
-      <c r="C35" s="2">
+      <c r="C35" s="1">
         <v>103627.382812</v>
       </c>
       <c r="D35">
@@ -4087,7 +4088,7 @@
       <c r="B36">
         <v>59793</v>
       </c>
-      <c r="C36" s="2">
+      <c r="C36" s="1">
         <v>137139.90625</v>
       </c>
       <c r="D36">

</xml_diff>